<commit_message>
Updated Sprint1 start date.
</commit_message>
<xml_diff>
--- a/docs/sprintPlanning.xlsx
+++ b/docs/sprintPlanning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\UF\ufCompSciOnline\spring2020\CEN3031\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\UF\ufCompSciOnline\spring2020\CEN3031\project\career-finder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD60DA6-BB63-4E29-9D9B-73DD5434BDBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F72BD0-74F0-4E0D-84F3-6553A4245127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6765" yWindow="1785" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baselineReqs" sheetId="5" r:id="rId1"/>
@@ -93,9 +93,6 @@
     <t>Client Interface</t>
   </si>
   <si>
-    <t>Add 3 APIs</t>
-  </si>
-  <si>
     <t>Full stack web app runs at provided URL. Updates at each sprint.</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>Client can easily update content on web app.</t>
   </si>
   <si>
-    <t>Utilize 3 Web APIs to enhance functionality. Ex: payment processing, scheduling, mapping, social media</t>
-  </si>
-  <si>
     <t>notes:</t>
   </si>
   <si>
@@ -184,6 +178,12 @@
   </si>
   <si>
     <t>weeksRemaining</t>
+  </si>
+  <si>
+    <t>Add 2 APIs</t>
+  </si>
+  <si>
+    <t>Utilize 2 Web APIs to enhance functionality. Ex: payment processing, scheduling, mapping, social media</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -495,13 +495,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C09444-FBF4-4B96-B4BC-41AE9BED77C0}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +852,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -876,7 +876,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -884,7 +884,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -892,7 +892,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -900,7 +900,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -908,7 +908,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -916,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -924,7 +924,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,15 +932,15 @@
         <v>17</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E2AA70-0FF3-4079-8445-A97303575861}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,10 +978,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -991,7 +991,7 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="25">
-        <v>43878</v>
+        <v>43885</v>
       </c>
       <c r="E2" s="26">
         <v>43900</v>
@@ -1002,13 +1002,13 @@
       </c>
       <c r="G2" s="22">
         <f ca="1" xml:space="preserve"> MOD(($E2 - TODAY()),7)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="27"/>
@@ -1018,7 +1018,7 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="29"/>
@@ -1027,7 +1027,7 @@
     <row r="5" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="27"/>
@@ -1037,7 +1037,7 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="29"/>
@@ -1046,7 +1046,7 @@
     <row r="7" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="27"/>
@@ -1056,7 +1056,7 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="31"/>
@@ -1080,13 +1080,13 @@
       </c>
       <c r="G9" s="22">
         <f ca="1" xml:space="preserve"> MOD(($E9 - TODAY()),7)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="27"/>
@@ -1097,7 +1097,7 @@
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="28"/>
@@ -1107,7 +1107,7 @@
       <c r="A12" s="12"/>
       <c r="B12" s="13"/>
       <c r="C12" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="28"/>
@@ -1116,7 +1116,7 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="29"/>
@@ -1125,7 +1125,7 @@
     <row r="14" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="27"/>
@@ -1135,7 +1135,7 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="31"/>
@@ -1159,13 +1159,13 @@
       </c>
       <c r="G16" s="22">
         <f ca="1" xml:space="preserve"> MOD(($E16 - TODAY()),7)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="33"/>
@@ -1175,7 +1175,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="35"/>
@@ -1184,7 +1184,7 @@
     <row r="19" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="33"/>
@@ -1194,7 +1194,7 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="37"/>

</xml_diff>